<commit_message>
Move add favourite call to utils class
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\applied-it-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02109DDB-02CA-4B7C-8CA3-C76DFE6E3569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAB5BBC-C22A-4933-AA12-82669141884D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="90" windowWidth="10875" windowHeight="10770" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,13 +490,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -518,12 +511,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -554,7 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,22 +561,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4233E53E-ADFE-474C-B1E0-EC32AE4CABC4}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -923,7 +928,7 @@
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -987,13 +992,13 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1234,13 +1239,13 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="8" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1488,7 +1493,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="mailto:trademe.test.login@gmail.com" xr:uid="{99178D11-3FAA-49E8-909F-9C1186F520FC}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{99178D11-3FAA-49E8-909F-9C1186F520FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Add delete favourites tests
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\applied-it-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAB5BBC-C22A-4933-AA12-82669141884D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA0BF9-35B9-4C04-A72B-7A0BFAD41C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="15165" windowHeight="10770" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,12 +290,6 @@
     <t>The new search is saved successfully</t>
   </si>
   <si>
-    <t>A client has an invalid search string</t>
-  </si>
-  <si>
-    <t>The response indicates that the search string is invalid</t>
-  </si>
-  <si>
     <t>A client has a valid search string
 And the search is already saved to the users account</t>
   </si>
@@ -455,6 +449,12 @@
   </si>
   <si>
     <t>The client sends a request to retrieve favourites from the TradeMe Favourites API without the details in the Authorization header</t>
+  </si>
+  <si>
+    <t>A client has an invalid search string and invalid search type</t>
+  </si>
+  <si>
+    <t>The response indicates that the search is invalid</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +521,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,7 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -583,6 +589,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -902,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4233E53E-ADFE-474C-B1E0-EC32AE4CABC4}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:C38"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1250,245 +1259,245 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B40" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="C40" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="5" t="s">
+    </row>
+    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="B41" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="C41" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="5" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="5" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B44" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="C44" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="5" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="5" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="C46" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="B47" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B48" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="B49" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="C49" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="5" t="s">
+    </row>
+    <row r="50" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="B50" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="C50" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="5" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C51" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B51" s="5" t="s">
+    <row r="52" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="5" t="s">
+    <row r="53" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C53" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" s="5" t="s">
+    <row r="54" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="B54" s="8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="C54" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B54" s="5" t="s">
+    </row>
+    <row r="55" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C55" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="5" t="s">
+    <row r="56" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="57" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C57" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="5" t="s">
+    <row r="58" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C58" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58" s="5" t="s">
+    <row r="59" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="C59" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="C60" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up flaky tests
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\applied-it-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA0BF9-35B9-4C04-A72B-7A0BFAD41C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F35EC-D1AC-488F-8863-4E7F7C2076A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="30" windowWidth="15165" windowHeight="10770" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
   </bookViews>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4233E53E-ADFE-474C-B1E0-EC32AE4CABC4}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:C59"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1138,112 +1138,112 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="126" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="8" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1490,13 +1490,13 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="8" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Operational: Add API tests
* Move add favourite call to utils class

* Add tests for adding favourite search and favourite seller

* Add update favourite tests

* Add delete favourites tests

* Add retrieve favourites tests

* Clean up flaky tests

* Add missing spaces at end of files
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\applied-it-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02109DDB-02CA-4B7C-8CA3-C76DFE6E3569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F35EC-D1AC-488F-8863-4E7F7C2076A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="90" windowWidth="10875" windowHeight="10770" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="15165" windowHeight="10770" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,12 +290,6 @@
     <t>The new search is saved successfully</t>
   </si>
   <si>
-    <t>A client has an invalid search string</t>
-  </si>
-  <si>
-    <t>The response indicates that the search string is invalid</t>
-  </si>
-  <si>
     <t>A client has a valid search string
 And the search is already saved to the users account</t>
   </si>
@@ -455,13 +449,19 @@
   </si>
   <si>
     <t>The client sends a request to retrieve favourites from the TradeMe Favourites API without the details in the Authorization header</t>
+  </si>
+  <si>
+    <t>A client has an invalid search string and invalid search type</t>
+  </si>
+  <si>
+    <t>The response indicates that the search is invalid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,13 +490,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -518,12 +511,24 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -554,7 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,22 +567,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4233E53E-ADFE-474C-B1E0-EC32AE4CABC4}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -923,7 +937,7 @@
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -987,13 +1001,13 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1124,371 +1138,371 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="126" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B40" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="C40" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="5" t="s">
+    </row>
+    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="B41" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="C41" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="5" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="5" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B44" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="C44" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="5" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="5" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="C46" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="B47" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B48" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="B49" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="C49" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="5" t="s">
+    </row>
+    <row r="50" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="B50" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="C50" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="5" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C51" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B51" s="5" t="s">
+    <row r="52" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="5" t="s">
+    <row r="53" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C53" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" s="5" t="s">
+    <row r="54" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="B54" s="8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="C54" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B54" s="5" t="s">
+    </row>
+    <row r="55" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C55" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="5" t="s">
+    <row r="56" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="57" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C57" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="5" t="s">
+    <row r="58" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C58" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58" s="5" t="s">
+    <row r="59" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C59" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="mailto:trademe.test.login@gmail.com" xr:uid="{99178D11-3FAA-49E8-909F-9C1186F520FC}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{99178D11-3FAA-49E8-909F-9C1186F520FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Implement the UI delete favourite tests
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\PL\Major requirements\Applied IT Project\applied-it-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F35EC-D1AC-488F-8863-4E7F7C2076A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25604A4-F4B8-41E9-AC22-588F5F6014B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="30" windowWidth="15165" windowHeight="10770" xr2:uid="{BD5E9B11-6A6A-451A-B8CD-2195B44E1030}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>The seller is saved in the seller tab</t>
   </si>
   <si>
-    <t>The category is saved in the seller tab</t>
-  </si>
-  <si>
     <t>Then the new update frequency is saved successfully</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>The response indicates that the search is invalid</t>
+  </si>
+  <si>
+    <t>The category is saved in the category tab</t>
   </si>
 </sst>
 </file>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4233E53E-ADFE-474C-B1E0-EC32AE4CABC4}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:C60"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -986,7 +986,7 @@
     </row>
     <row r="11" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,118 +1012,118 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="C15" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="C17" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="C20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="C21" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1139,365 +1139,365 @@
     </row>
     <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="C32" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="C35" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="126" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="C40" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="C48" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>